<commit_message>
Add TestCase column to dietician excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+  <si>
+    <t>TestCase</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -46,6 +49,9 @@
     <t>HospitalCity</t>
   </si>
   <si>
+    <t>FULL</t>
+  </si>
+  <si>
     <t>JohnFull</t>
   </si>
   <si>
@@ -76,6 +82,9 @@
     <t>HospitalCity 1</t>
   </si>
   <si>
+    <t>MANDATORY</t>
+  </si>
+  <si>
     <t>JohnMandatory</t>
   </si>
   <si>
@@ -106,6 +115,9 @@
     <t>HospitalCity 2</t>
   </si>
   <si>
+    <t>ADDITIONAL</t>
+  </si>
+  <si>
     <t>3333333333</t>
   </si>
   <si>
@@ -134,6 +146,9 @@
   </si>
   <si>
     <t>HospitalCity 3</t>
+  </si>
+  <si>
+    <t>INVALID</t>
   </si>
   <si>
     <t>JohnInvalidPincode</t>
@@ -1364,23 +1379,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.1719" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1719" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.1719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1719" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1417,139 +1432,154 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="3">
-        <v>11</v>
-      </c>
+      <c r="A2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>22</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" t="s" s="3">
-        <v>21</v>
-      </c>
+      <c r="A3" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s" s="3">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="L3" t="s" s="3">
+        <v>33</v>
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
       <c r="A4" t="s" s="4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s" s="4">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s" s="4">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s" s="4">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s" s="4">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s" s="4">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s" s="4">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s" s="4">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="L4" t="s" s="4">
+        <v>44</v>
       </c>
     </row>
     <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" t="s" s="5">
-        <v>41</v>
-      </c>
+      <c r="A5" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" t="s" s="5">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s" s="5">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s" s="5">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s" s="5">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s" s="5">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="L5" t="s" s="5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create dietician to use in GetById test and validate
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
   <si>
     <t>TestCase</t>
   </si>
@@ -179,6 +179,72 @@
   </si>
   <si>
     <t>HospitalCity 4</t>
+  </si>
+  <si>
+    <t>GET_BY_ID</t>
+  </si>
+  <si>
+    <t>JohnGetById</t>
+  </si>
+  <si>
+    <t>DoeGetById</t>
+  </si>
+  <si>
+    <t>5555555555</t>
+  </si>
+  <si>
+    <t>johndoegetbyid@gmail.com</t>
+  </si>
+  <si>
+    <t>1905-05-05T05:05:05.555Z</t>
+  </si>
+  <si>
+    <t>Education 5</t>
+  </si>
+  <si>
+    <t>HospitalName 5</t>
+  </si>
+  <si>
+    <t>HospitalStreet 5</t>
+  </si>
+  <si>
+    <t>555555</t>
+  </si>
+  <si>
+    <t>HospitalCity 5</t>
+  </si>
+  <si>
+    <t>GET_ALL</t>
+  </si>
+  <si>
+    <t>JohnGetAll</t>
+  </si>
+  <si>
+    <t>DoeGetAll</t>
+  </si>
+  <si>
+    <t>6666666666</t>
+  </si>
+  <si>
+    <t>johndoegetall@gmail.com</t>
+  </si>
+  <si>
+    <t>1906-06-06T06:06:06.666Z</t>
+  </si>
+  <si>
+    <t>Education 6</t>
+  </si>
+  <si>
+    <t>HospitalName 6</t>
+  </si>
+  <si>
+    <t>HospitalStreet 6</t>
+  </si>
+  <si>
+    <t>666666</t>
+  </si>
+  <si>
+    <t>HospitalCity 6</t>
   </si>
 </sst>
 </file>
@@ -231,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -284,21 +350,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -321,7 +372,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1379,7 +1430,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1582,6 +1633,78 @@
         <v>55</v>
       </c>
     </row>
+    <row r="6" ht="20.25" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" t="s" s="4">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s" s="4">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s" s="4">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s" s="4">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s" s="4">
+        <v>74</v>
+      </c>
+      <c r="J7" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s" s="4">
+        <v>76</v>
+      </c>
+      <c r="L7" t="s" s="4">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Create dietician to use in DeleteById test and validate
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>TestCase</t>
   </si>
@@ -245,6 +245,39 @@
   </si>
   <si>
     <t>HospitalCity 6</t>
+  </si>
+  <si>
+    <t>DELETE_BY_ID</t>
+  </si>
+  <si>
+    <t>JohnDeleteById</t>
+  </si>
+  <si>
+    <t>DoeDeleteById</t>
+  </si>
+  <si>
+    <t>7777777777</t>
+  </si>
+  <si>
+    <t>johndoedeletebyid@gmail.com</t>
+  </si>
+  <si>
+    <t>1907-07-07T07:07:07.777Z</t>
+  </si>
+  <si>
+    <t>Education 7</t>
+  </si>
+  <si>
+    <t>HospitalName 7</t>
+  </si>
+  <si>
+    <t>HospitalStreet 7</t>
+  </si>
+  <si>
+    <t>777777</t>
+  </si>
+  <si>
+    <t>HospitalCity 7</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1463,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1670,39 +1703,75 @@
       </c>
     </row>
     <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="A7" t="s" s="3">
         <v>67</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" t="s" s="4">
+      <c r="B7" s="3"/>
+      <c r="C7" t="s" s="3">
         <v>68</v>
       </c>
-      <c r="D7" t="s" s="4">
+      <c r="D7" t="s" s="3">
         <v>69</v>
       </c>
-      <c r="E7" t="s" s="4">
+      <c r="E7" t="s" s="3">
         <v>70</v>
       </c>
-      <c r="F7" t="s" s="4">
+      <c r="F7" t="s" s="3">
         <v>71</v>
       </c>
-      <c r="G7" t="s" s="4">
+      <c r="G7" t="s" s="3">
         <v>72</v>
       </c>
-      <c r="H7" t="s" s="4">
+      <c r="H7" t="s" s="3">
         <v>73</v>
       </c>
-      <c r="I7" t="s" s="4">
+      <c r="I7" t="s" s="3">
         <v>74</v>
       </c>
-      <c r="J7" t="s" s="4">
+      <c r="J7" t="s" s="3">
         <v>75</v>
       </c>
-      <c r="K7" t="s" s="4">
+      <c r="K7" t="s" s="3">
         <v>76</v>
       </c>
-      <c r="L7" t="s" s="4">
+      <c r="L7" t="s" s="3">
         <v>77</v>
+      </c>
+    </row>
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="A8" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" t="s" s="4">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s" s="4">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s" s="4">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s" s="4">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s" s="4">
+        <v>83</v>
+      </c>
+      <c r="H8" t="s" s="4">
+        <v>84</v>
+      </c>
+      <c r="I8" t="s" s="4">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s" s="4">
+        <v>86</v>
+      </c>
+      <c r="K8" t="s" s="4">
+        <v>87</v>
+      </c>
+      <c r="L8" t="s" s="4">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all dietician requests
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagar\Team7\AssuredTitan-Team7\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B035D5-B01C-4DD8-BF22-334C6D385211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077740DF-DF6F-4C09-A515-7F513622254F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>TestCase</t>
   </si>
@@ -79,21 +79,9 @@
     <t>MANDATORY</t>
   </si>
   <si>
-    <t>JohnMandatory</t>
-  </si>
-  <si>
     <t>DoeMandatory</t>
   </si>
   <si>
-    <t>2222222222</t>
-  </si>
-  <si>
-    <t>johndoemandatory@gmail.com</t>
-  </si>
-  <si>
-    <t>1902-02-02T02:02:02.222Z</t>
-  </si>
-  <si>
     <t>Education 2</t>
   </si>
   <si>
@@ -115,18 +103,9 @@
     <t>3333333333</t>
   </si>
   <si>
-    <t>JohnAdditional</t>
-  </si>
-  <si>
     <t>DoeAdditional</t>
   </si>
   <si>
-    <t>johndoeadditional@gmail.com</t>
-  </si>
-  <si>
-    <t>1903-03-03T03:03:03.333Z</t>
-  </si>
-  <si>
     <t>Education 3</t>
   </si>
   <si>
@@ -145,21 +124,9 @@
     <t>INVALID</t>
   </si>
   <si>
-    <t>JohnInvalidPincode</t>
-  </si>
-  <si>
     <t>DoeInvalidPincode</t>
   </si>
   <si>
-    <t>4444444444</t>
-  </si>
-  <si>
-    <t>johndoeinvalid@gmail.com</t>
-  </si>
-  <si>
-    <t>1904-04-04T04:04:04.444Z</t>
-  </si>
-  <si>
     <t>Education 4</t>
   </si>
   <si>
@@ -175,19 +142,55 @@
     <t>HospitalCity 4</t>
   </si>
   <si>
-    <t>JohnaFull</t>
-  </si>
-  <si>
     <t>DoeaFull</t>
   </si>
   <si>
-    <t>1111111234</t>
-  </si>
-  <si>
-    <t>johnasdoefull@gmail.com</t>
-  </si>
-  <si>
-    <t>1912-01-01T01:01:01.111Z</t>
+    <t>JohnaFulla</t>
+  </si>
+  <si>
+    <t>1234553356</t>
+  </si>
+  <si>
+    <t>john12doefull@gmail.com</t>
+  </si>
+  <si>
+    <t>1912-01-06T01:01:01.111Z</t>
+  </si>
+  <si>
+    <t>JohnaMandatory</t>
+  </si>
+  <si>
+    <t>JohnaAdditional</t>
+  </si>
+  <si>
+    <t>JohnaInvalidPincode</t>
+  </si>
+  <si>
+    <t>2222222212</t>
+  </si>
+  <si>
+    <t>3333333323</t>
+  </si>
+  <si>
+    <t>4444444434</t>
+  </si>
+  <si>
+    <t>johndoe1mandatory@gmail.com</t>
+  </si>
+  <si>
+    <t>johndoea1dditional@gmail.com</t>
+  </si>
+  <si>
+    <t>johndoe1invalid@gmail.com</t>
+  </si>
+  <si>
+    <t>1903-02-02T02:02:02.222Z</t>
+  </si>
+  <si>
+    <t>1902-03-03T03:03:03.333Z</t>
+  </si>
+  <si>
+    <t>1902-04-04T04:04:04.444Z</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -330,6 +333,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1469,7 +1478,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -1532,19 +1541,19 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>13</v>
@@ -1568,113 +1577,116 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{119C368E-4433-4910-A690-5A4D8C965016}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{3176F41E-47FC-4660-8135-59DE766D5993}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{AF66BC03-4E7A-4518-A047-6AF7C390A830}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{30554F13-99C4-48B6-9448-E3699ED1AFB0}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Changes in Excel Reader class -Resolving Null pointer exception
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagar\Team7\AssuredTitan-Team7\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\AssuredTitan-Team7\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444731A7-6BC4-468B-A3DF-A956A72D1C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFFD137-14D7-4654-9642-F78EDA78678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-9615" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dietician" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>TestCase</t>
   </si>
@@ -148,27 +148,9 @@
     <t>DoeFull</t>
   </si>
   <si>
-    <t>1111111111</t>
-  </si>
-  <si>
-    <t>johndoefull@gmail.com</t>
-  </si>
-  <si>
-    <t>1901-01-01T01:01:01.111Z</t>
-  </si>
-  <si>
     <t>JohnMandatory</t>
   </si>
   <si>
-    <t>2222222222</t>
-  </si>
-  <si>
-    <t>johndoemandatory@gmail.com</t>
-  </si>
-  <si>
-    <t>1902-02-02T02:02:02.222Z</t>
-  </si>
-  <si>
     <t>JohnAdditional</t>
   </si>
   <si>
@@ -287,13 +269,31 @@
   </si>
   <si>
     <t>HospitalCity 7</t>
+  </si>
+  <si>
+    <t>1144567893</t>
+  </si>
+  <si>
+    <t>2254422256</t>
+  </si>
+  <si>
+    <t>johndoe36mandatory@gmail.com</t>
+  </si>
+  <si>
+    <t>johndoe25full@gmail.com</t>
+  </si>
+  <si>
+    <t>1978-01-08T01:01:01.111Z</t>
+  </si>
+  <si>
+    <t>1983-02-15T02:02:02.222Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -303,6 +303,12 @@
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -380,12 +386,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -404,8 +413,12 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1537,10 +1550,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -1559,7 +1572,7 @@
     <col min="14" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1">
+    <row r="1" spans="1:12" ht="20.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1597,81 +1610,79 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="20.25" customHeight="1">
+    <row r="2" spans="1:12" ht="20.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>42</v>
+        <v>83</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="20.25" customHeight="1">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>84</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.25" customHeight="1">
+    <row r="4" spans="1:12" ht="20.25" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -1679,188 +1690,185 @@
         <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="20.25" customHeight="1">
+    <row r="5" spans="1:12" ht="20.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.95" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>39</v>
+      <c r="H6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="19.95" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="3" t="s">
+    <row r="7" spans="1:12" ht="19.95" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="H7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="19.95" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="3" t="s">
+    <row r="8" spans="1:12" ht="19.95" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="19.95" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{6C4DEB7D-D9F9-4E1A-AE23-BC254C96E686}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{F537E25D-CBB1-4773-83F4-144E868DF0A3}"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Pushing the merged  code
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/dietician.xlsx
+++ b/src/test/resources/ExcelData/dietician.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manal_\git\AssuredTitan-Team7\src\test\resources\ExcelData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA20C8C-FF95-4F3F-A82F-0E72D90B2A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9615" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Dietician" sheetId="1" r:id="rId1"/>
+    <sheet name="Dietician" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>TestCase</t>
   </si>
@@ -28,6 +19,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
     <t>Firstname</t>
   </si>
   <si>
@@ -61,6 +55,21 @@
     <t>FULL</t>
   </si>
   <si>
+    <t>JohnFull</t>
+  </si>
+  <si>
+    <t>DoeFull</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>johndoefull@gmail.com</t>
+  </si>
+  <si>
+    <t>1901-01-01T01:01:01.111Z</t>
+  </si>
+  <si>
     <t>Education 1</t>
   </si>
   <si>
@@ -79,9 +88,21 @@
     <t>MANDATORY</t>
   </si>
   <si>
+    <t>JohnMandatory</t>
+  </si>
+  <si>
     <t>DoeMandatory</t>
   </si>
   <si>
+    <t>2222222222</t>
+  </si>
+  <si>
+    <t>johndoemandatory@gmail.com</t>
+  </si>
+  <si>
+    <t>1902-02-02T02:02:02.222Z</t>
+  </si>
+  <si>
     <t>Education 2</t>
   </si>
   <si>
@@ -103,9 +124,18 @@
     <t>3333333333</t>
   </si>
   <si>
+    <t>JohnAdditional</t>
+  </si>
+  <si>
     <t>DoeAdditional</t>
   </si>
   <si>
+    <t>johndoeadditional@gmail.com</t>
+  </si>
+  <si>
+    <t>1903-03-03T03:03:03.333Z</t>
+  </si>
+  <si>
     <t>Education 3</t>
   </si>
   <si>
@@ -124,9 +154,21 @@
     <t>INVALID</t>
   </si>
   <si>
+    <t>JohnInvalidPincode</t>
+  </si>
+  <si>
     <t>DoeInvalidPincode</t>
   </si>
   <si>
+    <t>4444444444</t>
+  </si>
+  <si>
+    <t>johndoeinvalid@gmail.com</t>
+  </si>
+  <si>
+    <t>1904-04-04T04:04:04.444Z</t>
+  </si>
+  <si>
     <t>Education 4</t>
   </si>
   <si>
@@ -142,36 +184,6 @@
     <t>HospitalCity 4</t>
   </si>
   <si>
-    <t>JohnFull</t>
-  </si>
-  <si>
-    <t>DoeFull</t>
-  </si>
-  <si>
-    <t>JohnMandatory</t>
-  </si>
-  <si>
-    <t>JohnAdditional</t>
-  </si>
-  <si>
-    <t>johndoeadditional@gmail.com</t>
-  </si>
-  <si>
-    <t>1903-03-03T03:03:03.333Z</t>
-  </si>
-  <si>
-    <t>JohnInvalidPincode</t>
-  </si>
-  <si>
-    <t>4444444444</t>
-  </si>
-  <si>
-    <t>johndoeinvalid@gmail.com</t>
-  </si>
-  <si>
-    <t>1904-04-04T04:04:04.444Z</t>
-  </si>
-  <si>
     <t>GET_BY_ID</t>
   </si>
   <si>
@@ -271,44 +283,80 @@
     <t>HospitalCity 7</t>
   </si>
   <si>
-    <t>1144567892</t>
-  </si>
-  <si>
-    <t>johndoe26full@gmail.com</t>
-  </si>
-  <si>
-    <t>1978-01-09T01:01:01.111Z</t>
-  </si>
-  <si>
-    <t>2254422257</t>
-  </si>
-  <si>
-    <t>johndoe37mandatory@gmail.com</t>
-  </si>
-  <si>
-    <t>1983-02-16T02:02:02.222Z</t>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>JohnLogin</t>
+  </si>
+  <si>
+    <t>DoeLogin</t>
+  </si>
+  <si>
+    <t>8888888888</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>johndoelogin@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>1908-08-08T08:08:08.888Z</t>
+  </si>
+  <si>
+    <t>Education 8</t>
+  </si>
+  <si>
+    <t>HospitalName 8</t>
+  </si>
+  <si>
+    <t>HospitalStreet 8</t>
+  </si>
+  <si>
+    <t>888888</t>
+  </si>
+  <si>
+    <t>HospitalCity 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -332,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -385,125 +433,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFBDC0BF"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF3F3F3F"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -705,7 +769,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -723,7 +787,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -752,7 +816,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -777,7 +841,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -802,7 +866,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -827,7 +891,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -852,7 +916,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +941,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -902,7 +966,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +991,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -952,7 +1016,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -965,15 +1029,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -990,7 +1048,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1008,7 +1066,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1091,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,7 +1116,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,7 +1141,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1108,7 +1166,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,7 +1191,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1158,7 +1216,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1183,7 +1241,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1266,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1233,7 +1291,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1246,15 +1304,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1268,7 +1320,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1286,7 +1338,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1367,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1340,7 +1392,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1365,7 +1417,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1442,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1467,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,7 +1492,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1465,7 +1517,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1490,7 +1542,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1515,7 +1567,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1528,349 +1580,417 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="12.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24.21875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.33203125" style="1"/>
+    <col min="1" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6719" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6719" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1719" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1719" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>13</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="I4" t="s" s="4">
         <v>41</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="J4" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" ht="20.25" customHeight="1">
+      <c r="A5" t="s" s="5">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" t="s" s="5">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s" s="5">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s" s="5">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s" s="5">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s" s="5">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="L5" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="M5" t="s" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" ht="20.25" customHeight="1">
+      <c r="A6" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="L6" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" t="s" s="3">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s" s="3">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s" s="3">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s" s="3">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s" s="3">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s" s="3">
+        <v>74</v>
+      </c>
+      <c r="J7" t="s" s="3">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="L7" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="M7" t="s" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s" s="3">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s" s="3">
         <v>83</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="H8" t="s" s="3">
         <v>84</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I8" t="s" s="3">
         <v>85</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>17</v>
+      <c r="J8" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="K8" t="s" s="3">
+        <v>87</v>
+      </c>
+      <c r="L8" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="M8" t="s" s="3">
+        <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>24</v>
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="A9" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s" s="4">
+        <v>93</v>
+      </c>
+      <c r="G9" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s" s="4">
+        <v>95</v>
+      </c>
+      <c r="I9" t="s" s="4">
+        <v>96</v>
+      </c>
+      <c r="J9" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s" s="4">
+        <v>99</v>
+      </c>
+      <c r="M9" t="s" s="4">
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>32</v>
-      </c>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="19.95" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="19.95" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="19.95" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>82</v>
-      </c>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{6C4DEB7D-D9F9-4E1A-AE23-BC254C96E686}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{F537E25D-CBB1-4773-83F4-144E868DF0A3}"/>
+    <hyperlink ref="G9" r:id="rId1" location="" tooltip="" display="johndoelogin@gmail.com"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>